<commit_message>
Wired together but not spitting out excel yet
</commit_message>
<xml_diff>
--- a/src/test/resources/minimalProblemAndSolution.xlsx
+++ b/src/test/resources/minimalProblemAndSolution.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="candidate_preferences" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Bugs Bunny</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>period 2</t>
+  </si>
+  <si>
+    <t>Ginger</t>
   </si>
 </sst>
 </file>
@@ -381,12 +384,12 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -430,7 +433,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -455,7 +458,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
@@ -487,7 +490,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correlation read and a new soft constraint added to reduce the correlated allocations.
</commit_message>
<xml_diff>
--- a/src/test/resources/minimalProblemAndSolution.xlsx
+++ b/src/test/resources/minimalProblemAndSolution.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="15255" windowHeight="6990" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="candidate_preferences" sheetId="1" r:id="rId1"/>
     <sheet name="timetable" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="correlation" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Bugs Bunny</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Ginger</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test2</t>
   </si>
 </sst>
 </file>
@@ -383,8 +389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,12 +492,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reading key values and weights and mapping. The readers are ugly, will need to think how to make them nicer.
</commit_message>
<xml_diff>
--- a/src/test/resources/minimalProblemAndSolution.xlsx
+++ b/src/test/resources/minimalProblemAndSolution.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="15255" windowHeight="6990" activeTab="2"/>
+    <workbookView xWindow="1335" yWindow="300" windowWidth="15255" windowHeight="6990" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="candidate_preferences" sheetId="1" r:id="rId1"/>
     <sheet name="timetable" sheetId="2" r:id="rId2"/>
     <sheet name="correlation" sheetId="3" r:id="rId3"/>
+    <sheet name="key_values" sheetId="4" r:id="rId4"/>
+    <sheet name="weights" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Bugs Bunny</t>
   </si>
@@ -49,19 +51,76 @@
   </si>
   <si>
     <t>Test2</t>
+  </si>
+  <si>
+    <t>shiftsPerStudent</t>
+  </si>
+  <si>
+    <t>studentsPerShift</t>
+  </si>
+  <si>
+    <t>maxPreferences</t>
+  </si>
+  <si>
+    <t>groupSizeSoft</t>
+  </si>
+  <si>
+    <t>groupSizeHard</t>
+  </si>
+  <si>
+    <t>noOverlapping</t>
+  </si>
+  <si>
+    <t>noSimilar</t>
+  </si>
+  <si>
+    <t>correlation</t>
+  </si>
+  <si>
+    <t>longExperiment</t>
+  </si>
+  <si>
+    <t>preferences</t>
+  </si>
+  <si>
+    <t>preference1</t>
+  </si>
+  <si>
+    <t>preference2</t>
+  </si>
+  <si>
+    <t>preference3</t>
+  </si>
+  <si>
+    <t>preference4</t>
+  </si>
+  <si>
+    <t>preference5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -84,8 +143,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
@@ -530,4 +591,155 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Summary write simplified, but still need a test.
</commit_message>
<xml_diff>
--- a/src/test/resources/minimalProblemAndSolution.xlsx
+++ b/src/test/resources/minimalProblemAndSolution.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="300" windowWidth="15255" windowHeight="6990" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="13590" windowHeight="6690" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="candidate_preferences" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,8 @@
     <sheet name="key_values" sheetId="4" r:id="rId4"/>
     <sheet name="weights" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:M20"/>
 </workbook>
 </file>
 
@@ -555,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +599,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
The super simple shift reader test and the test instance that includes shifts.
</commit_message>
<xml_diff>
--- a/src/test/resources/minimalProblemAndSolution.xlsx
+++ b/src/test/resources/minimalProblemAndSolution.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="13590" windowHeight="6690" activeTab="2"/>
+    <workbookView xWindow="765" yWindow="1890" windowWidth="13590" windowHeight="6690" tabRatio="753" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="candidate_preferences" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="correlation" sheetId="3" r:id="rId3"/>
     <sheet name="key_values" sheetId="4" r:id="rId4"/>
     <sheet name="weights" sheetId="5" r:id="rId5"/>
+    <sheet name="periods" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1:M20"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Bugs Bunny</t>
   </si>
@@ -97,6 +97,36 @@
   </si>
   <si>
     <t>preference5</t>
+  </si>
+  <si>
+    <t>Period length</t>
+  </si>
+  <si>
+    <t>starting periods (separate and end in comma)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>1,</t>
+  </si>
+  <si>
+    <t>2,</t>
+  </si>
+  <si>
+    <t>3,</t>
   </si>
 </sst>
 </file>
@@ -144,10 +174,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,22 +530,28 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -556,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -743,4 +780,84 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="45.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>